<commit_message>
basic one line processing, object-wise
</commit_message>
<xml_diff>
--- a/geet-gatiroop/oo design.xlsx
+++ b/geet-gatiroop/oo design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vani-www\rhythmin-verse\geet-gatiroop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8FF8D9-4520-4A71-8BC3-E4316770D309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C640527-88C1-4B8A-829D-1A89BA84CE52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A2B0FDD6-85A7-463F-A27B-D34F39EE552C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>vis</t>
   </si>
@@ -147,14 +147,32 @@
     <t>poemLines[]</t>
   </si>
   <si>
-    <t>charCode</t>
+    <t>vowelChar</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>vowelNumber</t>
+  </si>
+  <si>
+    <t>mainChar</t>
+  </si>
+  <si>
+    <t>consonantNumber</t>
+  </si>
+  <si>
+    <t>hindiChar</t>
+  </si>
+  <si>
+    <t>inherited from: hindiChar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,7 +181,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -171,15 +190,21 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -206,11 +231,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,164 +557,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38FCFCB-E9FD-4D1B-BBF6-3FD0CAF1525E}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="J5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="H6" t="s">
+      <c r="J6" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H8" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H9" s="5" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>